<commit_message>
Add RG-0002: Kings of the Forest 1892 antique book
- Info card with flip card interaction
- QR code linking to Square payment
- Gallery index updated (2 items, era range 1890s-1980s)
- Label format reference added to rg-inventory skill
- Batch label files updated with SKU/QR columns
</commit_message>
<xml_diff>
--- a/rg-labels-batch.xlsx
+++ b/rg-labels-batch.xlsx
@@ -1,126 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Attributes</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Condition Notes</t>
-  </si>
-  <si>
-    <t>Little Orphan Annie 1930s Comic Strip Collection</t>
-  </si>
-  <si>
-    <t>Kings of the Forest &amp; Kindred Tribes - W.A. Foster</t>
-  </si>
-  <si>
-    <t>Pressed-Back Oak Swivel Bar Stool</t>
-  </si>
-  <si>
-    <t>Chase Japan Four Seasons Wall Plaque Set (4pc)</t>
-  </si>
-  <si>
-    <t>Chicago Bears 1985 World Champions Button on Card</t>
-  </si>
-  <si>
-    <t>Walt Disney's Comics and Stories Cover - May 1944 (Framed)</t>
-  </si>
-  <si>
-    <t>Dover Reprint • 1979 • Harold Gray</t>
-  </si>
-  <si>
-    <t>Antique Book • 1892 • 235 Engravings</t>
-  </si>
-  <si>
-    <t>Oak • Swivel • 1990s Repro</t>
-  </si>
-  <si>
-    <t>MCM Ceramic • Hand Painted • 1950s</t>
-  </si>
-  <si>
-    <t>NFL Licensed • Wincraft • 6" Pin</t>
-  </si>
-  <si>
-    <t>WWII Era • Walt Kelly Art • Donald Duck</t>
-  </si>
-  <si>
-    <t>VG</t>
-  </si>
-  <si>
-    <t>Fair</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Like New</t>
-  </si>
-  <si>
-    <t>Light cover wear, pages bright</t>
-  </si>
-  <si>
-    <t>Cover worn, spine frayed, pages intact</t>
-  </si>
-  <si>
-    <t>Working swivel</t>
-  </si>
-  <si>
-    <t>No chips/cracks</t>
-  </si>
-  <si>
-    <t>Card creased, button clean, slight fade</t>
-  </si>
-  <si>
-    <t>Cover only, professionally framed</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -135,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -451,133 +420,251 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Attributes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Condition Notes</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SKU</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>QR Code URL</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Little Orphan Annie 1930s Comic Strip Collection</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dover Reprint - 1979 - Harold Gray</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>19.99</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Light cover wear, pages bright</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>RG-0001</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://square.link/u/xn1pWPw6</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kings of the Forest &amp; Kindred Tribes - W.A. Foster</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Antique Book - 1892 - 235 Engravings</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>34.99</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fair</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Cover worn, spine frayed, pages intact</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>RG-0002</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://square.link/u/aug0H4mL</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pressed-Back Oak Swivel Bar Stool</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Oak - Swivel - 1990s Repro</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Working swivel</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>RG-0003</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Chase Japan Four Seasons Wall Plaque Set (4pc)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MCM Ceramic - Hand Painted - 1950s</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>69.98999999999999</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Like New</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No chips/cracks</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>RG-0004</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Chicago Bears 1985 World Champions Button on Card</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NFL Licensed - Wincraft - 6in Pin</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>12.99</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Card creased, button clean, slight fade</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>RG-0005</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Walt Disneys Comics and Stories Cover - May 1944 (Framed)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WWII Era - Walt Kelly Art - Donald Duck</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>49.99</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Cover only, professionally framed</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>RG-0006</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>